<commit_message>
Updated Excel with 100 emails
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\MailAccountCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA20A2F-2AD0-47DF-B206-CE18F5367AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FD8934-4C52-4446-BA63-07A3CDBE8BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>yeroc21795@galotv.com</t>
   </si>
@@ -268,6 +268,63 @@
   </si>
   <si>
     <t>jafama9018@anlubi.com</t>
+  </si>
+  <si>
+    <t>tigiti5067@logodez.com</t>
+  </si>
+  <si>
+    <t>hacitix414@galotv.com</t>
+  </si>
+  <si>
+    <t>piceliv680@aregods.com</t>
+  </si>
+  <si>
+    <t>layibo2375@logodez.com</t>
+  </si>
+  <si>
+    <t>hofipe3792@aregods.com</t>
+  </si>
+  <si>
+    <t>rirafit478@galotv.com</t>
+  </si>
+  <si>
+    <t>jegose7340@agrolivana.com</t>
+  </si>
+  <si>
+    <t>bosiko9979@logodez.com</t>
+  </si>
+  <si>
+    <t>wepop45766@logodez.com</t>
+  </si>
+  <si>
+    <t>hobac45491@anlubi.com</t>
+  </si>
+  <si>
+    <t>mamof13690@logodez.com</t>
+  </si>
+  <si>
+    <t>hejasen756@aregods.com</t>
+  </si>
+  <si>
+    <t>xojok63578@anlubi.com</t>
+  </si>
+  <si>
+    <t>lefeto3502@chimpad.com</t>
+  </si>
+  <si>
+    <t>jedila9621@agrolivana.com</t>
+  </si>
+  <si>
+    <t>vabedij950@chimpad.com</t>
+  </si>
+  <si>
+    <t>kicoxi2152@galotv.com</t>
+  </si>
+  <si>
+    <t>xoleb73061@chimpad.com</t>
+  </si>
+  <si>
+    <t>gahew87920@anlubi.com</t>
   </si>
 </sst>
 </file>
@@ -600,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A81"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,6 +1073,106 @@
         <v>80</v>
       </c>
     </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
300 Mails generated & Added to Data.xlsx
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivak\OneDrive\Documents\GitHub\MailCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F7FB44-84BB-453E-AC29-C8F7824E78DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F7B391-80C8-43EB-BC24-2A309897F1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="551">
   <si>
     <t>yeroc21795@galotv.com</t>
   </si>
@@ -328,13 +328,1363 @@
   </si>
   <si>
     <t>SIN</t>
+  </si>
+  <si>
+    <t>vitas39904@aregods.com</t>
+  </si>
+  <si>
+    <t>tehele4883@logodez.com</t>
+  </si>
+  <si>
+    <t>xobebe9507@logodez.com</t>
+  </si>
+  <si>
+    <t>xekofol967@anlubi.com</t>
+  </si>
+  <si>
+    <t>semeni9770@5k2u.com</t>
+  </si>
+  <si>
+    <t>wexehos424@galotv.com</t>
+  </si>
+  <si>
+    <t>digebax619@chimpad.com</t>
+  </si>
+  <si>
+    <t>codohok938@altpano.com</t>
+  </si>
+  <si>
+    <t>javos27653@chimpad.com</t>
+  </si>
+  <si>
+    <t>raxode8452@5k2u.com</t>
+  </si>
+  <si>
+    <t>sofolos652@anlubi.com</t>
+  </si>
+  <si>
+    <t>pinefo1283@logodez.com</t>
+  </si>
+  <si>
+    <t>wowerar246@chimpad.com</t>
+  </si>
+  <si>
+    <t>mepec31051@altpano.com</t>
+  </si>
+  <si>
+    <t>pofap20534@logodez.com</t>
+  </si>
+  <si>
+    <t>tahexe7225@anlubi.com</t>
+  </si>
+  <si>
+    <t>beveh22957@5k2u.com</t>
+  </si>
+  <si>
+    <t>vewajok530@anlubi.com</t>
+  </si>
+  <si>
+    <t>witex88321@aregods.com</t>
+  </si>
+  <si>
+    <t>relegol515@5k2u.com</t>
+  </si>
+  <si>
+    <t>sokokit119@agrolivana.com</t>
+  </si>
+  <si>
+    <t>pojov10421@chimpad.com</t>
+  </si>
+  <si>
+    <t>dovap37909@agrolivana.com</t>
+  </si>
+  <si>
+    <t>monepa5318@chimpad.com</t>
+  </si>
+  <si>
+    <t>vajas48401@logodez.com</t>
+  </si>
+  <si>
+    <t>vihix79824@aregods.com</t>
+  </si>
+  <si>
+    <t>kirac11797@galotv.com</t>
+  </si>
+  <si>
+    <t>lecec49198@agrolivana.com</t>
+  </si>
+  <si>
+    <t>dahiva4096@chimpad.com</t>
+  </si>
+  <si>
+    <t>xahena8492@chimpad.com</t>
+  </si>
+  <si>
+    <t>fedaye6297@altpano.com</t>
+  </si>
+  <si>
+    <t>weyifi3090@anlubi.com</t>
+  </si>
+  <si>
+    <t>lepiwat484@aregods.com</t>
+  </si>
+  <si>
+    <t>tacev12158@anlubi.com</t>
+  </si>
+  <si>
+    <t>mesoco9537@aregods.com</t>
+  </si>
+  <si>
+    <t>mobono7053@anlubi.com</t>
+  </si>
+  <si>
+    <t>gecev12514@anlubi.com</t>
+  </si>
+  <si>
+    <t>woxic36302@logodez.com</t>
+  </si>
+  <si>
+    <t>licejin676@aregods.com</t>
+  </si>
+  <si>
+    <t>xixates809@anlubi.com</t>
+  </si>
+  <si>
+    <t>xafenam698@agrolivana.com</t>
+  </si>
+  <si>
+    <t>fafaro9625@logodez.com</t>
+  </si>
+  <si>
+    <t>biwaca4450@altpano.com</t>
+  </si>
+  <si>
+    <t>kebef95004@galotv.com</t>
+  </si>
+  <si>
+    <t>rikibij474@agrolivana.com</t>
+  </si>
+  <si>
+    <t>fifogij948@agrolivana.com</t>
+  </si>
+  <si>
+    <t>vowib64515@5k2u.com</t>
+  </si>
+  <si>
+    <t>beviw82718@agrolivana.com</t>
+  </si>
+  <si>
+    <t>tedogo7322@anlubi.com</t>
+  </si>
+  <si>
+    <t>medah66317@anlubi.com</t>
+  </si>
+  <si>
+    <t>nigel95179@chimpad.com</t>
+  </si>
+  <si>
+    <t>jacay28672@logodez.com</t>
+  </si>
+  <si>
+    <t>dodom96587@galotv.com</t>
+  </si>
+  <si>
+    <t>yegeh74455@agrolivana.com</t>
+  </si>
+  <si>
+    <t>melag39066@agrolivana.com</t>
+  </si>
+  <si>
+    <t>sarejad737@anlubi.com</t>
+  </si>
+  <si>
+    <t>yecaci9059@anlubi.com</t>
+  </si>
+  <si>
+    <t>yidib43992@agrolivana.com</t>
+  </si>
+  <si>
+    <t>kiwowod545@altpano.com</t>
+  </si>
+  <si>
+    <t>disiko7753@galotv.com</t>
+  </si>
+  <si>
+    <t>demawov976@aregods.com</t>
+  </si>
+  <si>
+    <t>tocex16966@5k2u.com</t>
+  </si>
+  <si>
+    <t>hepil13552@altpano.com</t>
+  </si>
+  <si>
+    <t>fekem37826@chimpad.com</t>
+  </si>
+  <si>
+    <t>lacikom970@chimpad.com</t>
+  </si>
+  <si>
+    <t>xitatag129@galotv.com</t>
+  </si>
+  <si>
+    <t>garem83113@anlubi.com</t>
+  </si>
+  <si>
+    <t>kemec81629@galotv.com</t>
+  </si>
+  <si>
+    <t>lokigay849@logodez.com</t>
+  </si>
+  <si>
+    <t>bibewe8979@chimpad.com</t>
+  </si>
+  <si>
+    <t>kiyik69279@logodez.com</t>
+  </si>
+  <si>
+    <t>cejaban476@5k2u.com</t>
+  </si>
+  <si>
+    <t>dokisi7739@logodez.com</t>
+  </si>
+  <si>
+    <t>wicilo2039@aregods.com</t>
+  </si>
+  <si>
+    <t>verog80999@logodez.com</t>
+  </si>
+  <si>
+    <t>rowabof484@5k2u.com</t>
+  </si>
+  <si>
+    <t>tocemav154@logodez.com</t>
+  </si>
+  <si>
+    <t>lejoyif711@agrolivana.com</t>
+  </si>
+  <si>
+    <t>woyij86715@altpano.com</t>
+  </si>
+  <si>
+    <t>tayefat232@anlubi.com</t>
+  </si>
+  <si>
+    <t>bekoce8135@agrolivana.com</t>
+  </si>
+  <si>
+    <t>loyorex263@chimpad.com</t>
+  </si>
+  <si>
+    <t>mesidan625@agrolivana.com</t>
+  </si>
+  <si>
+    <t>hobog27298@5k2u.com</t>
+  </si>
+  <si>
+    <t>pagac99029@5k2u.com</t>
+  </si>
+  <si>
+    <t>hidolo6116@altpano.com</t>
+  </si>
+  <si>
+    <t>posedom810@agrolivana.com</t>
+  </si>
+  <si>
+    <t>pegan34293@aregods.com</t>
+  </si>
+  <si>
+    <t>borip93360@galotv.com</t>
+  </si>
+  <si>
+    <t>jihake9436@anlubi.com</t>
+  </si>
+  <si>
+    <t>dolarow947@galotv.com</t>
+  </si>
+  <si>
+    <t>simid95420@anlubi.com</t>
+  </si>
+  <si>
+    <t>laboroy557@altpano.com</t>
+  </si>
+  <si>
+    <t>degih91996@aregods.com</t>
+  </si>
+  <si>
+    <t>wahek81763@5k2u.com</t>
+  </si>
+  <si>
+    <t>lagap43451@chimpad.com</t>
+  </si>
+  <si>
+    <t>reyage1289@agrolivana.com</t>
+  </si>
+  <si>
+    <t>gojoxi4654@chimpad.com</t>
+  </si>
+  <si>
+    <t>taved26406@altpano.com</t>
+  </si>
+  <si>
+    <t>pimof95255@logodez.com</t>
+  </si>
+  <si>
+    <t>fecos32089@altpano.com</t>
+  </si>
+  <si>
+    <t>ragahi5598@agrolivana.com</t>
+  </si>
+  <si>
+    <t>yajiw44673@anlubi.com</t>
+  </si>
+  <si>
+    <t>ranofi5459@altpano.com</t>
+  </si>
+  <si>
+    <t>hefayo8662@galotv.com</t>
+  </si>
+  <si>
+    <t>tonigi4871@agrolivana.com</t>
+  </si>
+  <si>
+    <t>lonane5604@galotv.com</t>
+  </si>
+  <si>
+    <t>vopaxak120@aregods.com</t>
+  </si>
+  <si>
+    <t>yikakem998@5k2u.com</t>
+  </si>
+  <si>
+    <t>mayafon538@galotv.com</t>
+  </si>
+  <si>
+    <t>mogoto5646@aregods.com</t>
+  </si>
+  <si>
+    <t>nosafa7342@logodez.com</t>
+  </si>
+  <si>
+    <t>xateli8312@logodez.com</t>
+  </si>
+  <si>
+    <t>jidemi4652@agrolivana.com</t>
+  </si>
+  <si>
+    <t>tacoc17836@5k2u.com</t>
+  </si>
+  <si>
+    <t>vohivap373@altpano.com</t>
+  </si>
+  <si>
+    <t>vohama8034@aregods.com</t>
+  </si>
+  <si>
+    <t>dexalo5489@aregods.com</t>
+  </si>
+  <si>
+    <t>vacaceb789@chimpad.com</t>
+  </si>
+  <si>
+    <t>locexof320@galotv.com</t>
+  </si>
+  <si>
+    <t>nirewi6781@altpano.com</t>
+  </si>
+  <si>
+    <t>yilod42132@5k2u.com</t>
+  </si>
+  <si>
+    <t>rocote8946@logodez.com</t>
+  </si>
+  <si>
+    <t>keraco4557@5k2u.com</t>
+  </si>
+  <si>
+    <t>jixem68110@altpano.com</t>
+  </si>
+  <si>
+    <t>gawano4512@logodez.com</t>
+  </si>
+  <si>
+    <t>fiberit586@galotv.com</t>
+  </si>
+  <si>
+    <t>cabot44635@chimpad.com</t>
+  </si>
+  <si>
+    <t>raxad88834@logodez.com</t>
+  </si>
+  <si>
+    <t>bifahe7300@chimpad.com</t>
+  </si>
+  <si>
+    <t>wiperi2510@5k2u.com</t>
+  </si>
+  <si>
+    <t>nesihel391@aregods.com</t>
+  </si>
+  <si>
+    <t>gatalas190@logodez.com</t>
+  </si>
+  <si>
+    <t>doxil85082@altpano.com</t>
+  </si>
+  <si>
+    <t>kawewa6489@5k2u.com</t>
+  </si>
+  <si>
+    <t>yosoc25039@agrolivana.com</t>
+  </si>
+  <si>
+    <t>wemaroj395@chimpad.com</t>
+  </si>
+  <si>
+    <t>sekarax708@logodez.com</t>
+  </si>
+  <si>
+    <t>wicahi2238@agrolivana.com</t>
+  </si>
+  <si>
+    <t>sofito4931@agrolivana.com</t>
+  </si>
+  <si>
+    <t>mimewi8696@galotv.com</t>
+  </si>
+  <si>
+    <t>yoreyew118@logodez.com</t>
+  </si>
+  <si>
+    <t>bogofo5059@altpano.com</t>
+  </si>
+  <si>
+    <t>cocok33420@agrolivana.com</t>
+  </si>
+  <si>
+    <t>capejin513@logodez.com</t>
+  </si>
+  <si>
+    <t>cowedon465@chimpad.com</t>
+  </si>
+  <si>
+    <t>poyax22275@agrolivana.com</t>
+  </si>
+  <si>
+    <t>xibop22127@galotv.com</t>
+  </si>
+  <si>
+    <t>robol19644@logodez.com</t>
+  </si>
+  <si>
+    <t>kajah31851@anlubi.com</t>
+  </si>
+  <si>
+    <t>kefey42432@logodez.com</t>
+  </si>
+  <si>
+    <t>namaj16927@chimpad.com</t>
+  </si>
+  <si>
+    <t>cefowev638@altpano.com</t>
+  </si>
+  <si>
+    <t>legawoy593@chimpad.com</t>
+  </si>
+  <si>
+    <t>datasib116@chimpad.com</t>
+  </si>
+  <si>
+    <t>yemisoy180@chimpad.com</t>
+  </si>
+  <si>
+    <t>sosohi2501@galotv.com</t>
+  </si>
+  <si>
+    <t>lixolo1188@altpano.com</t>
+  </si>
+  <si>
+    <t>powedew399@agrolivana.com</t>
+  </si>
+  <si>
+    <t>pohan49706@logodez.com</t>
+  </si>
+  <si>
+    <t>depop91390@chimpad.com</t>
+  </si>
+  <si>
+    <t>fonace1187@galotv.com</t>
+  </si>
+  <si>
+    <t>yeyel95475@5k2u.com</t>
+  </si>
+  <si>
+    <t>tapowe4978@altpano.com</t>
+  </si>
+  <si>
+    <t>fitat55705@chimpad.com</t>
+  </si>
+  <si>
+    <t>vakilag638@logodez.com</t>
+  </si>
+  <si>
+    <t>hesan88041@5k2u.com</t>
+  </si>
+  <si>
+    <t>gilavek858@chimpad.com</t>
+  </si>
+  <si>
+    <t>mofic18237@agrolivana.com</t>
+  </si>
+  <si>
+    <t>woweyic705@anlubi.com</t>
+  </si>
+  <si>
+    <t>towafa4030@chimpad.com</t>
+  </si>
+  <si>
+    <t>hijeto7056@chimpad.com</t>
+  </si>
+  <si>
+    <t>bajic74519@chimpad.com</t>
+  </si>
+  <si>
+    <t>norim14070@galotv.com</t>
+  </si>
+  <si>
+    <t>vabadad566@agrolivana.com</t>
+  </si>
+  <si>
+    <t>vehep95509@logodez.com</t>
+  </si>
+  <si>
+    <t>jivir24111@5k2u.com</t>
+  </si>
+  <si>
+    <t>lakas54998@anlubi.com</t>
+  </si>
+  <si>
+    <t>raxoga7034@chimpad.com</t>
+  </si>
+  <si>
+    <t>belewo6191@aregods.com</t>
+  </si>
+  <si>
+    <t>fadid93232@logodez.com</t>
+  </si>
+  <si>
+    <t>hevik58123@anlubi.com</t>
+  </si>
+  <si>
+    <t>faday80987@agrolivana.com</t>
+  </si>
+  <si>
+    <t>tenago7280@chimpad.com</t>
+  </si>
+  <si>
+    <t>ganaf65904@galotv.com</t>
+  </si>
+  <si>
+    <t>lidili7366@altpano.com</t>
+  </si>
+  <si>
+    <t>magepe6253@agrolivana.com</t>
+  </si>
+  <si>
+    <t>mavavos297@aregods.com</t>
+  </si>
+  <si>
+    <t>niloje1449@aregods.com</t>
+  </si>
+  <si>
+    <t>cadekog665@agrolivana.com</t>
+  </si>
+  <si>
+    <t>satoyi3155@logodez.com</t>
+  </si>
+  <si>
+    <t>panaxox227@anlubi.com</t>
+  </si>
+  <si>
+    <t>gigera8980@anlubi.com</t>
+  </si>
+  <si>
+    <t>dipala7468@agrolivana.com</t>
+  </si>
+  <si>
+    <t>vivabad190@5k2u.com</t>
+  </si>
+  <si>
+    <t>rogog85443@aregods.com</t>
+  </si>
+  <si>
+    <t>camig39265@chimpad.com</t>
+  </si>
+  <si>
+    <t>midoriv941@logodez.com</t>
+  </si>
+  <si>
+    <t>janiwij709@chimpad.com</t>
+  </si>
+  <si>
+    <t>kogawa4426@5k2u.com</t>
+  </si>
+  <si>
+    <t>bahede7596@agrolivana.com</t>
+  </si>
+  <si>
+    <t>rexel91675@anlubi.com</t>
+  </si>
+  <si>
+    <t>lonow56770@anlubi.com</t>
+  </si>
+  <si>
+    <t>jafivoj167@anlubi.com</t>
+  </si>
+  <si>
+    <t>yikekeh495@logodez.com</t>
+  </si>
+  <si>
+    <t>yasin23841@agrolivana.com</t>
+  </si>
+  <si>
+    <t>gafif76176@logodez.com</t>
+  </si>
+  <si>
+    <t>kifam73057@aregods.com</t>
+  </si>
+  <si>
+    <t>nayobaf874@galotv.com</t>
+  </si>
+  <si>
+    <t>noxil67387@5k2u.com</t>
+  </si>
+  <si>
+    <t>lewohem665@anlubi.com</t>
+  </si>
+  <si>
+    <t>pesenip886@chimpad.com</t>
+  </si>
+  <si>
+    <t>veboxan721@anlubi.com</t>
+  </si>
+  <si>
+    <t>xoviwe2357@aregods.com</t>
+  </si>
+  <si>
+    <t>biwatod128@altpano.com</t>
+  </si>
+  <si>
+    <t>catige6694@chimpad.com</t>
+  </si>
+  <si>
+    <t>relige5317@aregods.com</t>
+  </si>
+  <si>
+    <t>fibir91509@aregods.com</t>
+  </si>
+  <si>
+    <t>hetepac674@aregods.com</t>
+  </si>
+  <si>
+    <t>ciwiko8291@galotv.com</t>
+  </si>
+  <si>
+    <t>sejal46917@anlubi.com</t>
+  </si>
+  <si>
+    <t>hirar43908@agrolivana.com</t>
+  </si>
+  <si>
+    <t>kesama6620@logodez.com</t>
+  </si>
+  <si>
+    <t>jebih44034@agrolivana.com</t>
+  </si>
+  <si>
+    <t>sowagi8359@5k2u.com</t>
+  </si>
+  <si>
+    <t>leyope1428@logodez.com</t>
+  </si>
+  <si>
+    <t>meday96886@chimpad.com</t>
+  </si>
+  <si>
+    <t>tepal65922@chimpad.com</t>
+  </si>
+  <si>
+    <t>cilef34783@agrolivana.com</t>
+  </si>
+  <si>
+    <t>pataved215@anlubi.com</t>
+  </si>
+  <si>
+    <t>gilise5924@5k2u.com</t>
+  </si>
+  <si>
+    <t>lekesed596@agrolivana.com</t>
+  </si>
+  <si>
+    <t>kewaw74942@anlubi.com</t>
+  </si>
+  <si>
+    <t>xodowi8925@altpano.com</t>
+  </si>
+  <si>
+    <t>lexayi1684@aregods.com</t>
+  </si>
+  <si>
+    <t>xefiga7690@logodez.com</t>
+  </si>
+  <si>
+    <t>kicipi1633@aregods.com</t>
+  </si>
+  <si>
+    <t>leliga8517@logodez.com</t>
+  </si>
+  <si>
+    <t>yemij48708@chimpad.com</t>
+  </si>
+  <si>
+    <t>hivop76572@5k2u.com</t>
+  </si>
+  <si>
+    <t>ramito5217@logodez.com</t>
+  </si>
+  <si>
+    <t>fepiy61398@aregods.com</t>
+  </si>
+  <si>
+    <t>tihoda1678@chimpad.com</t>
+  </si>
+  <si>
+    <t>payoc56535@agrolivana.com</t>
+  </si>
+  <si>
+    <t>yaromod604@galotv.com</t>
+  </si>
+  <si>
+    <t>nexixaf317@agrolivana.com</t>
+  </si>
+  <si>
+    <t>hitojof102@altpano.com</t>
+  </si>
+  <si>
+    <t>xetawe8903@aregods.com</t>
+  </si>
+  <si>
+    <t>teloyi9349@logodez.com</t>
+  </si>
+  <si>
+    <t>payiti8693@altpano.com</t>
+  </si>
+  <si>
+    <t>pefigiv810@altpano.com</t>
+  </si>
+  <si>
+    <t>biyodi2840@anlubi.com</t>
+  </si>
+  <si>
+    <t>ximis12949@logodez.com</t>
+  </si>
+  <si>
+    <t>xicola7544@galotv.com</t>
+  </si>
+  <si>
+    <t>matonaw976@agrolivana.com</t>
+  </si>
+  <si>
+    <t>hifodi2265@chimpad.com</t>
+  </si>
+  <si>
+    <t>tasicij929@aregods.com</t>
+  </si>
+  <si>
+    <t>bepobos168@logodez.com</t>
+  </si>
+  <si>
+    <t>hatemay846@5k2u.com</t>
+  </si>
+  <si>
+    <t>wobarir659@chimpad.com</t>
+  </si>
+  <si>
+    <t>wetal63348@galotv.com</t>
+  </si>
+  <si>
+    <t>bikorob398@5k2u.com</t>
+  </si>
+  <si>
+    <t>rajeke1210@galotv.com</t>
+  </si>
+  <si>
+    <t>mokex75358@agrolivana.com</t>
+  </si>
+  <si>
+    <t>gocajey337@5k2u.com</t>
+  </si>
+  <si>
+    <t>bekos80917@chimpad.com</t>
+  </si>
+  <si>
+    <t>vehoren549@galotv.com</t>
+  </si>
+  <si>
+    <t>nosegi3640@aregods.com</t>
+  </si>
+  <si>
+    <t>maxafi9447@logodez.com</t>
+  </si>
+  <si>
+    <t>hocesat819@galotv.com</t>
+  </si>
+  <si>
+    <t>ximem52535@5k2u.com</t>
+  </si>
+  <si>
+    <t>milare6257@5k2u.com</t>
+  </si>
+  <si>
+    <t>xowiher655@agrolivana.com</t>
+  </si>
+  <si>
+    <t>loxet85504@chimpad.com</t>
+  </si>
+  <si>
+    <t>sakaja7079@logodez.com</t>
+  </si>
+  <si>
+    <t>lagon56549@galotv.com</t>
+  </si>
+  <si>
+    <t>kadaje5924@altpano.com</t>
+  </si>
+  <si>
+    <t>lipadec494@anlubi.com</t>
+  </si>
+  <si>
+    <t>yavanek464@logodez.com</t>
+  </si>
+  <si>
+    <t>pewilo5898@agrolivana.com</t>
+  </si>
+  <si>
+    <t>xetop36266@galotv.com</t>
+  </si>
+  <si>
+    <t>fojoh71603@altpano.com</t>
+  </si>
+  <si>
+    <t>timow70604@altpano.com</t>
+  </si>
+  <si>
+    <t>dafohi6057@agrolivana.com</t>
+  </si>
+  <si>
+    <t>picovig840@chimpad.com</t>
+  </si>
+  <si>
+    <t>meroyit736@chimpad.com</t>
+  </si>
+  <si>
+    <t>vebohot349@5k2u.com</t>
+  </si>
+  <si>
+    <t>xixoneb482@aregods.com</t>
+  </si>
+  <si>
+    <t>gixega6199@anlubi.com</t>
+  </si>
+  <si>
+    <t>xoyip55750@chimpad.com</t>
+  </si>
+  <si>
+    <t>tamowi6269@chimpad.com</t>
+  </si>
+  <si>
+    <t>mojiy68825@galotv.com</t>
+  </si>
+  <si>
+    <t>licari1076@logodez.com</t>
+  </si>
+  <si>
+    <t>sorotol709@chimpad.com</t>
+  </si>
+  <si>
+    <t>lagak45696@galotv.com</t>
+  </si>
+  <si>
+    <t>hihile4061@chimpad.com</t>
+  </si>
+  <si>
+    <t>gafeci8541@logodez.com</t>
+  </si>
+  <si>
+    <t>doper97985@galotv.com</t>
+  </si>
+  <si>
+    <t>rideja4439@agrolivana.com</t>
+  </si>
+  <si>
+    <t>gokovas332@anlubi.com</t>
+  </si>
+  <si>
+    <t>yecow10315@altpano.com</t>
+  </si>
+  <si>
+    <t>remima1355@chimpad.com</t>
+  </si>
+  <si>
+    <t>tobal87506@anlubi.com</t>
+  </si>
+  <si>
+    <t>ciyeko3930@galotv.com</t>
+  </si>
+  <si>
+    <t>vobokit160@aregods.com</t>
+  </si>
+  <si>
+    <t>ceban79537@aregods.com</t>
+  </si>
+  <si>
+    <t>tikefe8183@chimpad.com</t>
+  </si>
+  <si>
+    <t>fepinem811@altpano.com</t>
+  </si>
+  <si>
+    <t>hipoh56635@logodez.com</t>
+  </si>
+  <si>
+    <t>rebewa1400@anlubi.com</t>
+  </si>
+  <si>
+    <t>namol22286@anlubi.com</t>
+  </si>
+  <si>
+    <t>kohocab273@agrolivana.com</t>
+  </si>
+  <si>
+    <t>jodaxex484@altpano.com</t>
+  </si>
+  <si>
+    <t>honomo9853@agrolivana.com</t>
+  </si>
+  <si>
+    <t>derige5934@anlubi.com</t>
+  </si>
+  <si>
+    <t>wojawok504@aregods.com</t>
+  </si>
+  <si>
+    <t>lacir33187@aregods.com</t>
+  </si>
+  <si>
+    <t>reyiri6762@aregods.com</t>
+  </si>
+  <si>
+    <t>newohoc283@agrolivana.com</t>
+  </si>
+  <si>
+    <t>xojoyaw537@chimpad.com</t>
+  </si>
+  <si>
+    <t>boteba2721@galotv.com</t>
+  </si>
+  <si>
+    <t>yinobo9146@chimpad.com</t>
+  </si>
+  <si>
+    <t>jebema8649@aregods.com</t>
+  </si>
+  <si>
+    <t>javayi8069@logodez.com</t>
+  </si>
+  <si>
+    <t>bomobe6126@agrolivana.com</t>
+  </si>
+  <si>
+    <t>larof11296@agrolivana.com</t>
+  </si>
+  <si>
+    <t>walolal629@agrolivana.com</t>
+  </si>
+  <si>
+    <t>bixahim947@anlubi.com</t>
+  </si>
+  <si>
+    <t>piwepe4154@chimpad.com</t>
+  </si>
+  <si>
+    <t>nireki2864@logodez.com</t>
+  </si>
+  <si>
+    <t>rafeter352@galotv.com</t>
+  </si>
+  <si>
+    <t>gemiya9367@5k2u.com</t>
+  </si>
+  <si>
+    <t>fajon37717@5k2u.com</t>
+  </si>
+  <si>
+    <t>fedijop754@chimpad.com</t>
+  </si>
+  <si>
+    <t>pahex25671@aregods.com</t>
+  </si>
+  <si>
+    <t>kamecaf571@5k2u.com</t>
+  </si>
+  <si>
+    <t>vemowa9251@logodez.com</t>
+  </si>
+  <si>
+    <t>jafari3443@galotv.com</t>
+  </si>
+  <si>
+    <t>loxiroh729@5k2u.com</t>
+  </si>
+  <si>
+    <t>gemivic325@galotv.com</t>
+  </si>
+  <si>
+    <t>jorixoh632@altpano.com</t>
+  </si>
+  <si>
+    <t>denopeg918@5k2u.com</t>
+  </si>
+  <si>
+    <t>kayino4149@galotv.com</t>
+  </si>
+  <si>
+    <t>xetih46486@galotv.com</t>
+  </si>
+  <si>
+    <t>pasapa8193@altpano.com</t>
+  </si>
+  <si>
+    <t>vayibe1000@5k2u.com</t>
+  </si>
+  <si>
+    <t>nigad40888@5k2u.com</t>
+  </si>
+  <si>
+    <t>wirepip463@galotv.com</t>
+  </si>
+  <si>
+    <t>gesajoj331@5k2u.com</t>
+  </si>
+  <si>
+    <t>xojoka5022@aregods.com</t>
+  </si>
+  <si>
+    <t>ligonaf673@galotv.com</t>
+  </si>
+  <si>
+    <t>rekacoy316@5k2u.com</t>
+  </si>
+  <si>
+    <t>wowobo1980@altpano.com</t>
+  </si>
+  <si>
+    <t>kifajo3498@agrolivana.com</t>
+  </si>
+  <si>
+    <t>tejim95989@5k2u.com</t>
+  </si>
+  <si>
+    <t>dagam90982@agrolivana.com</t>
+  </si>
+  <si>
+    <t>pofixo8282@aregods.com</t>
+  </si>
+  <si>
+    <t>caxekad987@agrolivana.com</t>
+  </si>
+  <si>
+    <t>nasit95769@chimpad.com</t>
+  </si>
+  <si>
+    <t>videmi9771@5k2u.com</t>
+  </si>
+  <si>
+    <t>wekelep708@5k2u.com</t>
+  </si>
+  <si>
+    <t>tenayi2691@aregods.com</t>
+  </si>
+  <si>
+    <t>sogalin936@logodez.com</t>
+  </si>
+  <si>
+    <t>saheb30067@logodez.com</t>
+  </si>
+  <si>
+    <t>cibom87197@altpano.com</t>
+  </si>
+  <si>
+    <t>sakoja6591@galotv.com</t>
+  </si>
+  <si>
+    <t>bagofow553@logodez.com</t>
+  </si>
+  <si>
+    <t>motik80905@5k2u.com</t>
+  </si>
+  <si>
+    <t>resari7235@logodez.com</t>
+  </si>
+  <si>
+    <t>tejoco8294@agrolivana.com</t>
+  </si>
+  <si>
+    <t>pakali7147@altpano.com</t>
+  </si>
+  <si>
+    <t>refic56205@agrolivana.com</t>
+  </si>
+  <si>
+    <t>ceweka8276@anlubi.com</t>
+  </si>
+  <si>
+    <t>bapayo7618@chimpad.com</t>
+  </si>
+  <si>
+    <t>coyop11459@logodez.com</t>
+  </si>
+  <si>
+    <t>getepec693@altpano.com</t>
+  </si>
+  <si>
+    <t>memeh70990@logodez.com</t>
+  </si>
+  <si>
+    <t>fesowa2862@anlubi.com</t>
+  </si>
+  <si>
+    <t>socil32852@chimpad.com</t>
+  </si>
+  <si>
+    <t>cahon67958@anlubi.com</t>
+  </si>
+  <si>
+    <t>jomom63520@altpano.com</t>
+  </si>
+  <si>
+    <t>xideg13212@logodez.com</t>
+  </si>
+  <si>
+    <t>kemev72260@aregods.com</t>
+  </si>
+  <si>
+    <t>vahaso5080@anlubi.com</t>
+  </si>
+  <si>
+    <t>padovi3164@galotv.com</t>
+  </si>
+  <si>
+    <t>sesad19307@altpano.com</t>
+  </si>
+  <si>
+    <t>sepano2520@anlubi.com</t>
+  </si>
+  <si>
+    <t>kokiw85008@chimpad.com</t>
+  </si>
+  <si>
+    <t>cesic14399@anlubi.com</t>
+  </si>
+  <si>
+    <t>xehic74488@agrolivana.com</t>
+  </si>
+  <si>
+    <t>dibabeh298@galotv.com</t>
+  </si>
+  <si>
+    <t>cirixes361@anlubi.com</t>
+  </si>
+  <si>
+    <t>yogiy70925@altpano.com</t>
+  </si>
+  <si>
+    <t>gelip46314@5k2u.com</t>
+  </si>
+  <si>
+    <t>gijar99603@galotv.com</t>
+  </si>
+  <si>
+    <t>wanamox940@chimpad.com</t>
+  </si>
+  <si>
+    <t>kosaxe3224@logodez.com</t>
+  </si>
+  <si>
+    <t>ticofod306@anlubi.com</t>
+  </si>
+  <si>
+    <t>robono7933@5k2u.com</t>
+  </si>
+  <si>
+    <t>kolace1988@logodez.com</t>
+  </si>
+  <si>
+    <t>macofen220@agrolivana.com</t>
+  </si>
+  <si>
+    <t>nibamon239@logodez.com</t>
+  </si>
+  <si>
+    <t>tixopox541@logodez.com</t>
+  </si>
+  <si>
+    <t>hikowaj370@aregods.com</t>
+  </si>
+  <si>
+    <t>vopoma9789@galotv.com</t>
+  </si>
+  <si>
+    <t>tohoto6487@agrolivana.com</t>
+  </si>
+  <si>
+    <t>fofiy35935@logodez.com</t>
+  </si>
+  <si>
+    <t>pirid43947@5k2u.com</t>
+  </si>
+  <si>
+    <t>casetip342@agrolivana.com</t>
+  </si>
+  <si>
+    <t>yihep74330@anlubi.com</t>
+  </si>
+  <si>
+    <t>gifadik791@chimpad.com</t>
+  </si>
+  <si>
+    <t>tevomaw952@chimpad.com</t>
+  </si>
+  <si>
+    <t>girobof444@altpano.com</t>
+  </si>
+  <si>
+    <t>ciyadek930@logodez.com</t>
+  </si>
+  <si>
+    <t>tipew73127@altpano.com</t>
+  </si>
+  <si>
+    <t>recew79195@anlubi.com</t>
+  </si>
+  <si>
+    <t>ceboli3694@altpano.com</t>
+  </si>
+  <si>
+    <t>tihaja2168@aregods.com</t>
+  </si>
+  <si>
+    <t>xibihi1931@agrolivana.com</t>
+  </si>
+  <si>
+    <t>nemac39034@logodez.com</t>
+  </si>
+  <si>
+    <t>yekije5056@5k2u.com</t>
+  </si>
+  <si>
+    <t>tenot97082@agrolivana.com</t>
+  </si>
+  <si>
+    <t>nonorec119@anlubi.com</t>
+  </si>
+  <si>
+    <t>figihim329@chimpad.com</t>
+  </si>
+  <si>
+    <t>nojex96695@logodez.com</t>
+  </si>
+  <si>
+    <t>bolov61651@aregods.com</t>
+  </si>
+  <si>
+    <t>diyir98568@chimpad.com</t>
+  </si>
+  <si>
+    <t>xasaje3500@5k2u.com</t>
+  </si>
+  <si>
+    <t>noded95299@5k2u.com</t>
+  </si>
+  <si>
+    <t>xagapam593@chimpad.com</t>
+  </si>
+  <si>
+    <t>jajoboh915@logodez.com</t>
+  </si>
+  <si>
+    <t>bofimex794@anlubi.com</t>
+  </si>
+  <si>
+    <t>hopir12138@agrolivana.com</t>
+  </si>
+  <si>
+    <t>cabicok518@anlubi.com</t>
+  </si>
+  <si>
+    <t>tomam29112@chimpad.com</t>
+  </si>
+  <si>
+    <t>sibex40369@aregods.com</t>
+  </si>
+  <si>
+    <t>jowelay390@altpano.com</t>
+  </si>
+  <si>
+    <t>xexog12520@altpano.com</t>
+  </si>
+  <si>
+    <t>sevare6939@altpano.com</t>
+  </si>
+  <si>
+    <t>wekop84994@aregods.com</t>
+  </si>
+  <si>
+    <t>tositi4239@aregods.com</t>
+  </si>
+  <si>
+    <t>fawofe6630@altpano.com</t>
+  </si>
+  <si>
+    <t>mitor86315@logodez.com</t>
+  </si>
+  <si>
+    <t>xehah20810@logodez.com</t>
+  </si>
+  <si>
+    <t>sibopis742@galotv.com</t>
+  </si>
+  <si>
+    <t>hapeyib415@altpano.com</t>
+  </si>
+  <si>
+    <t>kexav29991@logodez.com</t>
+  </si>
+  <si>
+    <t>haxefo3862@logodez.com</t>
+  </si>
+  <si>
+    <t>cogige9868@agrolivana.com</t>
+  </si>
+  <si>
+    <t>fecovi5250@agrolivana.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +1696,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,9 +1734,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +2018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B551"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A518" workbookViewId="0">
+      <selection activeCell="A543" sqref="A543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,6 +2538,2256 @@
         <v>99</v>
       </c>
     </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>550</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>